<commit_message>
Update files and scripts for review
</commit_message>
<xml_diff>
--- a/output/continuous_simple_slopes_anova.xlsx
+++ b/output/continuous_simple_slopes_anova.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t xml:space="preserve">asrs_sum</t>
+    <t xml:space="preserve">frameref</t>
   </si>
   <si>
-    <t xml:space="preserve">frameref</t>
+    <t xml:space="preserve">asrs_sum</t>
   </si>
   <si>
     <t xml:space="preserve">fit</t>
@@ -415,11 +415,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="n">
         <v>4.8574647052353</v>
@@ -428,7 +428,7 @@
         <v>0.0809757442124169</v>
       </c>
       <c r="E2" t="n">
-        <v>4.69844967131587</v>
+        <v>4.69844967131586</v>
       </c>
       <c r="F2" t="n">
         <v>5.01647973915474</v>
@@ -438,195 +438,195 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.41541213281222</v>
+        <v>4.91644400749225</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.0809757442124169</v>
       </c>
       <c r="E3" t="n">
-        <v>4.31436198997489</v>
+        <v>4.75742897357281</v>
       </c>
       <c r="F3" t="n">
-        <v>4.51646227564954</v>
+        <v>5.07545904141169</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6.2</v>
       </c>
       <c r="C4" t="n">
-        <v>4.00187908119062</v>
+        <v>4.41541213281222</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0514580937244535</v>
       </c>
       <c r="E4" t="n">
-        <v>3.93876549211198</v>
+        <v>4.31436198997489</v>
       </c>
       <c r="F4" t="n">
-        <v>4.06499267026925</v>
+        <v>4.51646227564954</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6.2</v>
       </c>
       <c r="C5" t="n">
-        <v>3.50278746716455</v>
+        <v>4.58098775096866</v>
       </c>
       <c r="D5" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0514580937244535</v>
       </c>
       <c r="E5" t="n">
-        <v>3.42152235601373</v>
+        <v>4.47993760813133</v>
       </c>
       <c r="F5" t="n">
-        <v>3.58405257831537</v>
+        <v>4.68203789380598</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>3.07499465514221</v>
+        <v>4.00187908119062</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0321395387567471</v>
       </c>
       <c r="E6" t="n">
-        <v>2.94204745936882</v>
+        <v>3.93876549211198</v>
       </c>
       <c r="F6" t="n">
-        <v>3.20794185091559</v>
+        <v>4.06499267026925</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>4.91644400749225</v>
+        <v>4.26717383357562</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0321395387567471</v>
       </c>
       <c r="E7" t="n">
-        <v>4.75742897357281</v>
+        <v>4.20406024449698</v>
       </c>
       <c r="F7" t="n">
-        <v>5.07545904141169</v>
+        <v>4.33028742265425</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>4.58098775096866</v>
+        <v>3.50278746716455</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.041382897527014</v>
       </c>
       <c r="E8" t="n">
-        <v>4.47993760813133</v>
+        <v>3.42152235601373</v>
       </c>
       <c r="F8" t="n">
-        <v>4.68203789380599</v>
+        <v>3.58405257831537</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>19</v>
       </c>
       <c r="C9" t="n">
-        <v>4.26717383357562</v>
+        <v>3.88843289879091</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.041382897527014</v>
       </c>
       <c r="E9" t="n">
-        <v>4.20406024449698</v>
+        <v>3.80716778764009</v>
       </c>
       <c r="F9" t="n">
-        <v>4.33028742265425</v>
+        <v>3.96969800994174</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="n">
+        <v>25</v>
       </c>
       <c r="C10" t="n">
-        <v>3.88843289879091</v>
+        <v>3.07499465514221</v>
       </c>
       <c r="D10" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0677011339956571</v>
       </c>
       <c r="E10" t="n">
-        <v>3.80716778764009</v>
+        <v>2.94204745936882</v>
       </c>
       <c r="F10" t="n">
-        <v>3.96969800994174</v>
+        <v>3.20794185091559</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
       </c>
       <c r="C11" t="n">
         <v>3.5637978118326</v>
@@ -645,1380 +645,1380 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="n">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
       <c r="C12" t="n">
-        <v>4.8574647052353</v>
+        <v>4.87619946041916</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0851459751280406</v>
       </c>
       <c r="E12" t="n">
-        <v>4.69844967131587</v>
+        <v>4.70899519135345</v>
       </c>
       <c r="F12" t="n">
-        <v>5.01647973915474</v>
+        <v>5.04340372948487</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>4.41541213281222</v>
+        <v>4.91174418269944</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.0851459751280406</v>
       </c>
       <c r="E13" t="n">
-        <v>4.31436198997489</v>
+        <v>4.74453991363373</v>
       </c>
       <c r="F13" t="n">
-        <v>4.51646227564954</v>
+        <v>5.07894845176515</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6.2</v>
       </c>
       <c r="C14" t="n">
-        <v>4.00187908119062</v>
+        <v>4.53009956989563</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0541081728981112</v>
       </c>
       <c r="E14" t="n">
-        <v>3.93876549211198</v>
+        <v>4.42384536954964</v>
       </c>
       <c r="F14" t="n">
-        <v>4.06499267026925</v>
+        <v>4.63635377024162</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="n">
+        <v>6.2</v>
       </c>
       <c r="C15" t="n">
-        <v>3.50278746716455</v>
+        <v>4.65849924839153</v>
       </c>
       <c r="D15" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0541081728981112</v>
       </c>
       <c r="E15" t="n">
-        <v>3.42152235601373</v>
+        <v>4.55224504804553</v>
       </c>
       <c r="F15" t="n">
-        <v>3.58405257831537</v>
+        <v>4.76475344873752</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="n">
+        <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>3.07499465514221</v>
+        <v>4.20632870456717</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0337947170998526</v>
       </c>
       <c r="E16" t="n">
-        <v>2.94204745936882</v>
+        <v>4.13996478117013</v>
       </c>
       <c r="F16" t="n">
-        <v>3.20794185091559</v>
+        <v>4.27269262796421</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="n">
+        <v>12</v>
       </c>
       <c r="C17" t="n">
-        <v>4.91644400749225</v>
+        <v>4.42159269694219</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0337947170998526</v>
       </c>
       <c r="E17" t="n">
-        <v>4.75742897357281</v>
+        <v>4.35522877354515</v>
       </c>
       <c r="F17" t="n">
-        <v>5.07545904141169</v>
+        <v>4.48795662033923</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="n">
+        <v>19</v>
       </c>
       <c r="C18" t="n">
-        <v>4.58098775096866</v>
+        <v>3.81557076365351</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.043514106573918</v>
       </c>
       <c r="E18" t="n">
-        <v>4.47993760813133</v>
+        <v>3.73012051926089</v>
       </c>
       <c r="F18" t="n">
-        <v>4.68203789380599</v>
+        <v>3.90102100804613</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="n">
+        <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>4.26717383357562</v>
+        <v>4.13567099691713</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.043514106573918</v>
       </c>
       <c r="E19" t="n">
-        <v>4.20406024449698</v>
+        <v>4.0502207525245</v>
       </c>
       <c r="F19" t="n">
-        <v>4.33028742265425</v>
+        <v>4.22112124130975</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="n">
+        <v>25</v>
       </c>
       <c r="C20" t="n">
-        <v>3.88843289879091</v>
+        <v>3.48063538572752</v>
       </c>
       <c r="D20" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0711877257492439</v>
       </c>
       <c r="E20" t="n">
-        <v>3.80716778764009</v>
+        <v>3.3408414420625</v>
       </c>
       <c r="F20" t="n">
-        <v>3.96969800994174</v>
+        <v>3.62042932939254</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="n">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
       <c r="C21" t="n">
-        <v>3.5637978118326</v>
+        <v>3.8905952540385</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0711877257492438</v>
       </c>
       <c r="E21" t="n">
-        <v>3.43085061605921</v>
+        <v>3.75080131037348</v>
       </c>
       <c r="F21" t="n">
-        <v>3.69674500760598</v>
+        <v>4.03038919770353</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="n">
         <v>0</v>
       </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
       <c r="C22" t="n">
-        <v>4.8574647052353</v>
+        <v>4.87420382780168</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.14407031720576</v>
       </c>
       <c r="E22" t="n">
-        <v>4.69844967131587</v>
+        <v>4.59128767062303</v>
       </c>
       <c r="F22" t="n">
-        <v>5.01647973915474</v>
+        <v>5.15711998498033</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>4.41541213281222</v>
+        <v>4.95609029358876</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.14407031720576</v>
       </c>
       <c r="E23" t="n">
-        <v>4.31436198997489</v>
+        <v>4.67317413641011</v>
       </c>
       <c r="F23" t="n">
-        <v>4.51646227564954</v>
+        <v>5.23900645076741</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6.2</v>
       </c>
       <c r="C24" t="n">
-        <v>4.00187908119062</v>
+        <v>4.23599614120003</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0915531429539969</v>
       </c>
       <c r="E24" t="n">
-        <v>3.93876549211198</v>
+        <v>4.0562098820695</v>
       </c>
       <c r="F24" t="n">
-        <v>4.06499267026925</v>
+        <v>4.41578240033055</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="n">
+        <v>6.2</v>
       </c>
       <c r="C25" t="n">
-        <v>3.50278746716455</v>
+        <v>4.52135955848906</v>
       </c>
       <c r="D25" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0915531429539969</v>
       </c>
       <c r="E25" t="n">
-        <v>3.42152235601373</v>
+        <v>4.34157329935853</v>
       </c>
       <c r="F25" t="n">
-        <v>3.58405257831537</v>
+        <v>4.70114581761959</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="n">
+        <v>12</v>
       </c>
       <c r="C26" t="n">
-        <v>3.07499465514221</v>
+        <v>3.63896314405654</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0571819819449252</v>
       </c>
       <c r="E26" t="n">
-        <v>2.94204745936882</v>
+        <v>3.52667279233467</v>
       </c>
       <c r="F26" t="n">
-        <v>3.20794185091559</v>
+        <v>3.75125349577842</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="n">
+        <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>4.91644400749225</v>
+        <v>4.11467596758934</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0571819819449252</v>
       </c>
       <c r="E27" t="n">
-        <v>4.75742897357281</v>
+        <v>4.00238561586746</v>
       </c>
       <c r="F27" t="n">
-        <v>5.07545904141169</v>
+        <v>4.22696631931121</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="n">
+        <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>4.58098775096866</v>
+        <v>2.91840607853855</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.073627568744174</v>
       </c>
       <c r="E28" t="n">
-        <v>4.47993760813133</v>
+        <v>2.77382092584704</v>
       </c>
       <c r="F28" t="n">
-        <v>4.68203789380599</v>
+        <v>3.06299123123005</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
-        <v>9</v>
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="n">
+        <v>19</v>
       </c>
       <c r="C29" t="n">
-        <v>4.26717383357562</v>
+        <v>3.62385094408968</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0736275687441741</v>
       </c>
       <c r="E29" t="n">
-        <v>4.20406024449698</v>
+        <v>3.47926579139817</v>
       </c>
       <c r="F29" t="n">
-        <v>4.33028742265425</v>
+        <v>3.76843609678118</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>9</v>
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="n">
+        <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>3.88843289879091</v>
+        <v>2.30078573666598</v>
       </c>
       <c r="D30" t="n">
-        <v>0.041382897527014</v>
+        <v>0.120452413803792</v>
       </c>
       <c r="E30" t="n">
-        <v>3.80716778764009</v>
+        <v>2.06424892119141</v>
       </c>
       <c r="F30" t="n">
-        <v>3.96969800994174</v>
+        <v>2.53732255214055</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="n">
         <v>25</v>
       </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
       <c r="C31" t="n">
-        <v>3.5637978118326</v>
+        <v>3.20314378108997</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.120452413803792</v>
       </c>
       <c r="E31" t="n">
-        <v>3.43085061605921</v>
+        <v>2.9666069656154</v>
       </c>
       <c r="F31" t="n">
-        <v>3.69674500760598</v>
+        <v>3.43968059656453</v>
       </c>
       <c r="G31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="n">
         <v>0</v>
       </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
       <c r="C32" t="n">
-        <v>4.8574647052353</v>
+        <v>4.82539912130829</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0881974600813456</v>
       </c>
       <c r="E32" t="n">
-        <v>4.69844967131587</v>
+        <v>4.65220253950654</v>
       </c>
       <c r="F32" t="n">
-        <v>5.01647973915474</v>
+        <v>4.99859570311004</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4.95464744171427</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0881974600813456</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.78145085991252</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5.12784402351603</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="n">
         <v>6.2</v>
       </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="n">
-        <v>4.41541213281222</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.0514580937244535</v>
-      </c>
-      <c r="E33" t="n">
-        <v>4.31436198997489</v>
-      </c>
-      <c r="F33" t="n">
-        <v>4.51646227564954</v>
-      </c>
-      <c r="G33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
       <c r="C34" t="n">
-        <v>4.00187908119062</v>
+        <v>4.54430864518936</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0560473165299874</v>
       </c>
       <c r="E34" t="n">
-        <v>3.93876549211198</v>
+        <v>4.43424647748973</v>
       </c>
       <c r="F34" t="n">
-        <v>4.06499267026925</v>
+        <v>4.65437081288899</v>
       </c>
       <c r="G34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4.714327532408</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0560473165299873</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4.60426536470836</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.82438970010763</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="n">
+        <v>12</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4.28135303849745</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0350058614971819</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.21261074650009</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4.35009533049481</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="n">
+        <v>12</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4.48951213337954</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0350058614971819</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.42076984138218</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4.5582544253769</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="n">
         <v>19</v>
       </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="n">
-        <v>3.50278746716455</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.041382897527014</v>
-      </c>
-      <c r="E35" t="n">
-        <v>3.42152235601373</v>
-      </c>
-      <c r="F35" t="n">
-        <v>3.58405257831537</v>
-      </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
+      <c r="C38" t="n">
+        <v>3.96399282352446</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0450735771333573</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.87548018969266</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4.05250545735626</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="n">
+        <v>19</v>
+      </c>
+      <c r="C39" t="n">
+        <v>4.21818320351761</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0450735771333573</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.12967056968581</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4.30669583734941</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="n">
         <v>25</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="n">
-        <v>3.07499465514221</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.0677011339956571</v>
-      </c>
-      <c r="E36" t="n">
-        <v>2.94204745936882</v>
-      </c>
-      <c r="F36" t="n">
-        <v>3.20794185091559</v>
-      </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
+      <c r="C40" t="n">
+        <v>3.69196978211904</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0737389711094298</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.54716586452377</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3.83677369971431</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="n">
+        <v>25</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3.98561554935025</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0737389711094297</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.84081163175498</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.13041946694552</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="n">
         <v>0</v>
       </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" t="n">
-        <v>4.91644400749225</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.0809757442124169</v>
-      </c>
-      <c r="E37" t="n">
-        <v>4.75742897357281</v>
-      </c>
-      <c r="F37" t="n">
-        <v>5.07545904141169</v>
-      </c>
-      <c r="G37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" t="n">
-        <v>4.58098775096866</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.0514580937244535</v>
-      </c>
-      <c r="E38" t="n">
-        <v>4.47993760813133</v>
-      </c>
-      <c r="F38" t="n">
-        <v>4.68203789380599</v>
-      </c>
-      <c r="G38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" t="n">
-        <v>4.26717383357562</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.0321395387567471</v>
-      </c>
-      <c r="E39" t="n">
-        <v>4.20406024449698</v>
-      </c>
-      <c r="F39" t="n">
-        <v>4.33028742265425</v>
-      </c>
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" t="n">
-        <v>3.88843289879091</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.041382897527014</v>
-      </c>
-      <c r="E40" t="n">
-        <v>3.80716778764009</v>
-      </c>
-      <c r="F40" t="n">
-        <v>3.96969800994174</v>
-      </c>
-      <c r="G40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>25</v>
-      </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" t="n">
-        <v>3.5637978118326</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.0677011339956571</v>
-      </c>
-      <c r="E41" t="n">
-        <v>3.43085061605921</v>
-      </c>
-      <c r="F41" t="n">
-        <v>3.69674500760598</v>
-      </c>
-      <c r="G41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
       <c r="C42" t="n">
-        <v>4.8574647052353</v>
+        <v>4.64818463977139</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.114207537666644</v>
       </c>
       <c r="E42" t="n">
-        <v>4.69844967131587</v>
+        <v>4.42391111622986</v>
       </c>
       <c r="F42" t="n">
-        <v>5.01647973915474</v>
+        <v>4.87245816331293</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>4.41541213281222</v>
+        <v>4.59024542640922</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.114207537666644</v>
       </c>
       <c r="E43" t="n">
-        <v>4.31436198997489</v>
+        <v>4.36597190286769</v>
       </c>
       <c r="F43" t="n">
-        <v>4.51646227564954</v>
+        <v>4.81451894995076</v>
       </c>
       <c r="G43" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>12</v>
-      </c>
-      <c r="B44" t="s">
-        <v>7</v>
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="n">
+        <v>6.2</v>
       </c>
       <c r="C44" t="n">
-        <v>4.00187908119062</v>
+        <v>4.34026892069941</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0725760810777223</v>
       </c>
       <c r="E44" t="n">
-        <v>3.93876549211198</v>
+        <v>4.19774861283981</v>
       </c>
       <c r="F44" t="n">
-        <v>4.06499267026925</v>
+        <v>4.48278922855901</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>19</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="n">
+        <v>6.2</v>
       </c>
       <c r="C45" t="n">
-        <v>3.50278746716455</v>
+        <v>4.37419734535851</v>
       </c>
       <c r="D45" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0725760810777223</v>
       </c>
       <c r="E45" t="n">
-        <v>3.42152235601373</v>
+        <v>4.23167703749891</v>
       </c>
       <c r="F45" t="n">
-        <v>3.58405257831537</v>
+        <v>4.51671765321811</v>
       </c>
       <c r="G45" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>25</v>
-      </c>
-      <c r="B46" t="s">
-        <v>7</v>
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="n">
+        <v>12</v>
       </c>
       <c r="C46" t="n">
-        <v>3.07499465514221</v>
+        <v>4.05221873189014</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0453293466932682</v>
       </c>
       <c r="E46" t="n">
-        <v>2.94204745936882</v>
+        <v>3.96320383400827</v>
       </c>
       <c r="F46" t="n">
-        <v>3.20794185091559</v>
+        <v>4.141233629772</v>
       </c>
       <c r="G46" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
-        <v>9</v>
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="n">
+        <v>12</v>
       </c>
       <c r="C47" t="n">
-        <v>4.91644400749225</v>
+        <v>4.17208785018203</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0453293466932682</v>
       </c>
       <c r="E47" t="n">
-        <v>4.75742897357281</v>
+        <v>4.08307295230017</v>
       </c>
       <c r="F47" t="n">
-        <v>5.07545904141169</v>
+        <v>4.26110274806389</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>9</v>
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="n">
+        <v>19</v>
       </c>
       <c r="C48" t="n">
-        <v>4.58098775096866</v>
+        <v>3.70457195229274</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.0583661054805983</v>
       </c>
       <c r="E48" t="n">
-        <v>4.47993760813133</v>
+        <v>3.58995629382597</v>
       </c>
       <c r="F48" t="n">
-        <v>4.68203789380599</v>
+        <v>3.81918761075951</v>
       </c>
       <c r="G48" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>12</v>
-      </c>
-      <c r="B49" t="s">
-        <v>9</v>
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" t="n">
+        <v>19</v>
       </c>
       <c r="C49" t="n">
-        <v>4.26717383357562</v>
+        <v>3.92816259738283</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0583661054805983</v>
       </c>
       <c r="E49" t="n">
-        <v>4.20406024449698</v>
+        <v>3.81354693891606</v>
       </c>
       <c r="F49" t="n">
-        <v>4.33028742265425</v>
+        <v>4.0427782558496</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>19</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="n">
+        <v>25</v>
       </c>
       <c r="C50" t="n">
-        <v>3.88843289879091</v>
+        <v>3.40658899835211</v>
       </c>
       <c r="D50" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0954851342965299</v>
       </c>
       <c r="E50" t="n">
-        <v>3.80716778764009</v>
+        <v>3.21908134384837</v>
       </c>
       <c r="F50" t="n">
-        <v>3.96969800994174</v>
+        <v>3.59409665285584</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="n">
         <v>25</v>
       </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
       <c r="C51" t="n">
-        <v>3.5637978118326</v>
+        <v>3.71908380926924</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0954851342965299</v>
       </c>
       <c r="E51" t="n">
-        <v>3.43085061605921</v>
+        <v>3.5315761547655</v>
       </c>
       <c r="F51" t="n">
-        <v>3.69674500760598</v>
+        <v>3.90659146377297</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="n">
         <v>0</v>
       </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
       <c r="C52" t="n">
-        <v>4.8574647052353</v>
+        <v>4.86190778744119</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.113795723864997</v>
       </c>
       <c r="E52" t="n">
-        <v>4.69844967131587</v>
+        <v>4.63844295774093</v>
       </c>
       <c r="F52" t="n">
-        <v>5.01647973915474</v>
+        <v>5.08537261714145</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>4.41541213281222</v>
+        <v>4.95823729618577</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.113795723864997</v>
       </c>
       <c r="E53" t="n">
-        <v>4.31436198997489</v>
+        <v>4.73477246648551</v>
       </c>
       <c r="F53" t="n">
-        <v>4.51646227564954</v>
+        <v>5.18170212588603</v>
       </c>
       <c r="G53" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>12</v>
-      </c>
-      <c r="B54" t="s">
-        <v>7</v>
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="n">
+        <v>6.2</v>
       </c>
       <c r="C54" t="n">
-        <v>4.00187908119062</v>
+        <v>4.30572333416322</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0723143835359672</v>
       </c>
       <c r="E54" t="n">
-        <v>3.93876549211198</v>
+        <v>4.16371693134868</v>
       </c>
       <c r="F54" t="n">
-        <v>4.06499267026925</v>
+        <v>4.44772973697775</v>
       </c>
       <c r="G54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>19</v>
-      </c>
-      <c r="B55" t="s">
-        <v>7</v>
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="n">
+        <v>6.2</v>
       </c>
       <c r="C55" t="n">
-        <v>3.50278746716455</v>
+        <v>4.51077327660873</v>
       </c>
       <c r="D55" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0723143835359672</v>
       </c>
       <c r="E55" t="n">
-        <v>3.42152235601373</v>
+        <v>4.3687668737942</v>
       </c>
       <c r="F55" t="n">
-        <v>3.58405257831537</v>
+        <v>4.65277967942326</v>
       </c>
       <c r="G55" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>25</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="n">
+        <v>12</v>
       </c>
       <c r="C56" t="n">
-        <v>3.07499465514221</v>
+        <v>3.78542174883866</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0451658964432283</v>
       </c>
       <c r="E56" t="n">
-        <v>2.94204745936882</v>
+        <v>3.6967278241977</v>
       </c>
       <c r="F56" t="n">
-        <v>3.20794185091559</v>
+        <v>3.87411567347962</v>
       </c>
       <c r="G56" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>0</v>
-      </c>
-      <c r="B57" t="s">
-        <v>9</v>
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="n">
+        <v>12</v>
       </c>
       <c r="C57" t="n">
-        <v>4.91644400749225</v>
+        <v>4.09217790345602</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0451658964432284</v>
       </c>
       <c r="E57" t="n">
-        <v>4.75742897357281</v>
+        <v>4.00348397881505</v>
       </c>
       <c r="F57" t="n">
-        <v>5.07545904141169</v>
+        <v>4.18087182809698</v>
       </c>
       <c r="G57" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B58" t="s">
-        <v>9</v>
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="n">
+        <v>19</v>
       </c>
       <c r="C58" t="n">
-        <v>4.58098775096866</v>
+        <v>3.15747155965385</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.0581556467991783</v>
       </c>
       <c r="E58" t="n">
-        <v>4.47993760813133</v>
+        <v>3.04326918660594</v>
       </c>
       <c r="F58" t="n">
-        <v>4.68203789380599</v>
+        <v>3.27167393270175</v>
       </c>
       <c r="G58" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>12</v>
-      </c>
-      <c r="B59" t="s">
-        <v>9</v>
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" t="n">
+        <v>19</v>
       </c>
       <c r="C59" t="n">
-        <v>4.26717383357562</v>
+        <v>3.58697659103033</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0581556467991783</v>
       </c>
       <c r="E59" t="n">
-        <v>4.20406024449698</v>
+        <v>3.47277421798242</v>
       </c>
       <c r="F59" t="n">
-        <v>4.33028742265425</v>
+        <v>3.70117896407823</v>
       </c>
       <c r="G59" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>9</v>
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="n">
+        <v>25</v>
       </c>
       <c r="C60" t="n">
-        <v>3.88843289879091</v>
+        <v>2.61922854035258</v>
       </c>
       <c r="D60" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0951408304356895</v>
       </c>
       <c r="E60" t="n">
-        <v>3.80716778764009</v>
+        <v>2.43239700794741</v>
       </c>
       <c r="F60" t="n">
-        <v>3.96969800994174</v>
+        <v>2.80606007275775</v>
       </c>
       <c r="G60" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" t="n">
         <v>25</v>
       </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
       <c r="C61" t="n">
-        <v>3.5637978118326</v>
+        <v>3.15394689466545</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0951408304356895</v>
       </c>
       <c r="E61" t="n">
-        <v>3.43085061605921</v>
+        <v>2.96711536226028</v>
       </c>
       <c r="F61" t="n">
-        <v>3.69674500760598</v>
+        <v>3.34077842707062</v>
       </c>
       <c r="G61" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="n">
         <v>0</v>
       </c>
-      <c r="B62" t="s">
-        <v>7</v>
-      </c>
       <c r="C62" t="n">
-        <v>4.8574647052353</v>
+        <v>5.05392784368965</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.140835254052931</v>
       </c>
       <c r="E62" t="n">
-        <v>4.69844967131587</v>
+        <v>4.77736449847935</v>
       </c>
       <c r="F62" t="n">
-        <v>5.01647973915474</v>
+        <v>5.33049118889994</v>
       </c>
       <c r="G62" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B63" t="s">
-        <v>7</v>
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>4.41541213281222</v>
+        <v>5.1328046674828</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.140835254052931</v>
       </c>
       <c r="E63" t="n">
-        <v>4.31436198997489</v>
+        <v>4.8562413222725</v>
       </c>
       <c r="F63" t="n">
-        <v>4.51646227564954</v>
+        <v>5.4093680126931</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>12</v>
-      </c>
-      <c r="B64" t="s">
-        <v>7</v>
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="n">
+        <v>6.2</v>
       </c>
       <c r="C64" t="n">
-        <v>4.00187908119062</v>
+        <v>4.53394839871634</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0894973398917116</v>
       </c>
       <c r="E64" t="n">
-        <v>3.93876549211198</v>
+        <v>4.35819919533455</v>
       </c>
       <c r="F64" t="n">
-        <v>4.06499267026925</v>
+        <v>4.70969760209813</v>
       </c>
       <c r="G64" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>19</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="n">
+        <v>6.2</v>
       </c>
       <c r="C65" t="n">
-        <v>3.50278746716455</v>
+        <v>4.7099374326979</v>
       </c>
       <c r="D65" t="n">
-        <v>0.041382897527014</v>
+        <v>0.0894973398917116</v>
       </c>
       <c r="E65" t="n">
-        <v>3.42152235601373</v>
+        <v>4.53418822931611</v>
       </c>
       <c r="F65" t="n">
-        <v>3.58405257831537</v>
+        <v>4.8856866360797</v>
       </c>
       <c r="G65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>25</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="n">
+        <v>12</v>
       </c>
       <c r="C66" t="n">
-        <v>3.07499465514221</v>
+        <v>4.04751601470905</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.0558979747574417</v>
       </c>
       <c r="E66" t="n">
-        <v>2.94204745936882</v>
+        <v>3.93774711491647</v>
       </c>
       <c r="F66" t="n">
-        <v>3.20794185091559</v>
+        <v>4.15728491450163</v>
       </c>
       <c r="G66" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>0</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="n">
+        <v>12</v>
       </c>
       <c r="C67" t="n">
-        <v>4.91644400749225</v>
+        <v>4.3143519549959</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0809757442124169</v>
+        <v>0.0558979747574418</v>
       </c>
       <c r="E67" t="n">
-        <v>4.75742897357281</v>
+        <v>4.20458305520332</v>
       </c>
       <c r="F67" t="n">
-        <v>5.07545904141169</v>
+        <v>4.42412085478849</v>
       </c>
       <c r="G67" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="n">
+        <v>19</v>
       </c>
       <c r="C68" t="n">
-        <v>4.58098775096866</v>
+        <v>3.46044244780371</v>
       </c>
       <c r="D68" t="n">
-        <v>0.0514580937244535</v>
+        <v>0.0719742799939624</v>
       </c>
       <c r="E68" t="n">
-        <v>4.47993760813133</v>
+        <v>3.31910391876785</v>
       </c>
       <c r="F68" t="n">
-        <v>4.68203789380599</v>
+        <v>3.60178097683957</v>
       </c>
       <c r="G68" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>12</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" t="n">
+        <v>19</v>
       </c>
       <c r="C69" t="n">
-        <v>4.26717383357562</v>
+        <v>3.83692120604522</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0321395387567471</v>
+        <v>0.0719742799939624</v>
       </c>
       <c r="E69" t="n">
-        <v>4.20406024449698</v>
+        <v>3.69558267700936</v>
       </c>
       <c r="F69" t="n">
-        <v>4.33028742265425</v>
+        <v>3.97825973508108</v>
       </c>
       <c r="G69" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>19</v>
-      </c>
-      <c r="B70" t="s">
-        <v>9</v>
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="n">
+        <v>25</v>
       </c>
       <c r="C70" t="n">
-        <v>3.88843289879091</v>
+        <v>2.95723653331341</v>
       </c>
       <c r="D70" t="n">
-        <v>0.041382897527014</v>
+        <v>0.11774768479977</v>
       </c>
       <c r="E70" t="n">
-        <v>3.80716778764009</v>
+        <v>2.72601109322045</v>
       </c>
       <c r="F70" t="n">
-        <v>3.96969800994174</v>
+        <v>3.18846197340637</v>
       </c>
       <c r="G70" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" t="n">
         <v>25</v>
       </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
       <c r="C71" t="n">
-        <v>3.5637978118326</v>
+        <v>3.42769484980177</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0677011339956571</v>
+        <v>0.11774768479977</v>
       </c>
       <c r="E71" t="n">
-        <v>3.43085061605921</v>
+        <v>3.19646940970881</v>
       </c>
       <c r="F71" t="n">
-        <v>3.69674500760598</v>
+        <v>3.65892028989473</v>
       </c>
       <c r="G71" t="s">
         <v>15</v>

</xml_diff>